<commit_message>
Update Verisiones de war (ciclo solo Oracle).xlsx
</commit_message>
<xml_diff>
--- a/Verisiones de war (ciclo solo Oracle).xlsx
+++ b/Verisiones de war (ciclo solo Oracle).xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ManuelV\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git\turbus_web2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{404FCFF3-B6A8-4C87-8C30-BF54D83E889E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CFEBD59-D123-4FCD-B011-4F95FB843CAC}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6945" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="6945" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Pruebas funcionales DLS" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="39">
   <si>
     <t>Versión</t>
   </si>
@@ -119,9 +119,6 @@
   </si>
   <si>
     <t>ddls-1.8.9.war</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 13-02</t>
   </si>
   <si>
     <t xml:space="preserve"> 13-03</t>
@@ -140,6 +137,24 @@
   </si>
   <si>
     <t>600, 855, 854</t>
+  </si>
+  <si>
+    <t>ddls-1.8.10.war</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13-02 al 27-02</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 27-02 al 01-03</t>
+  </si>
+  <si>
+    <t>ddls-1.8.11.war</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 01-03</t>
+  </si>
+  <si>
+    <t>893, 899, 901, 902, 903, 904, 905, 912</t>
   </si>
 </sst>
 </file>
@@ -244,9 +259,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -276,6 +288,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -581,8 +596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A3:K33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,7 +639,7 @@
       <c r="A4">
         <v>1</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="12" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -647,7 +662,7 @@
       <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>15</v>
       </c>
       <c r="D5" s="6">
@@ -672,10 +687,10 @@
       <c r="A6">
         <v>3</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="15" t="s">
+      <c r="C6" s="14" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="6">
@@ -696,13 +711,13 @@
       <c r="A7">
         <v>4</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="C7" s="17" t="s">
+      <c r="C7" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="D7" s="20">
+      <c r="D7" s="19">
         <v>169</v>
       </c>
       <c r="E7" s="6">
@@ -717,11 +732,11 @@
       </c>
     </row>
     <row r="8" spans="1:11" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="21" t="s">
+      <c r="B8" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="21" t="s">
-        <v>28</v>
+      <c r="C8" s="20" t="s">
+        <v>34</v>
       </c>
       <c r="D8" s="6">
         <v>362</v>
@@ -736,30 +751,54 @@
         <v>16</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="9"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
+      <c r="B9" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="6">
+        <v>34</v>
+      </c>
+      <c r="E9" s="6">
+        <v>33</v>
+      </c>
+      <c r="F9" s="6">
+        <v>1</v>
+      </c>
       <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="3"/>
-      <c r="C10" s="10"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
+      <c r="H9" s="6">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D10" s="6">
+        <v>10</v>
+      </c>
+      <c r="E10" s="6">
+        <v>8</v>
+      </c>
+      <c r="F10" s="6">
+        <v>2</v>
+      </c>
       <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
+      <c r="H10" s="6" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B11" s="3"/>
-      <c r="C11" s="10"/>
+      <c r="C11" s="9"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
       <c r="F11" s="6"/>
@@ -817,7 +856,7 @@
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="8"/>
       <c r="C25" s="5"/>
-      <c r="H25" s="11"/>
+      <c r="H25" s="10"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="8"/>
@@ -864,8 +903,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4284620-DE89-4C68-A6A4-FA228134A475}">
   <dimension ref="B3:I18"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -885,25 +924,25 @@
       <c r="F3" s="26"/>
     </row>
     <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C4" s="18" t="s">
+      <c r="C4" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="19" t="s">
+      <c r="D4" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="18" t="s">
         <v>12</v>
       </c>
     </row>
@@ -911,10 +950,10 @@
       <c r="B5">
         <v>1</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="15" t="s">
         <v>13</v>
       </c>
       <c r="E5" s="6">
@@ -931,10 +970,10 @@
       <c r="B6">
         <v>2</v>
       </c>
-      <c r="C6" s="16" t="s">
+      <c r="C6" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="15" t="s">
         <v>15</v>
       </c>
       <c r="E6" s="6">
@@ -955,10 +994,10 @@
       <c r="B7" s="4">
         <v>3</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="21" t="s">
         <v>23</v>
       </c>
       <c r="E7" s="6">
@@ -979,13 +1018,13 @@
       <c r="B8">
         <v>4</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="22" t="s">
+      <c r="D8" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E8" s="20">
+      <c r="E8" s="19">
         <v>169</v>
       </c>
       <c r="F8" s="6">
@@ -1003,17 +1042,17 @@
       <c r="B9" s="4">
         <v>5</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="21" t="s">
         <v>27</v>
       </c>
       <c r="D9" s="22" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E9" s="6">
-        <v>340</v>
+        <v>362</v>
       </c>
       <c r="F9" s="6">
-        <v>301</v>
+        <v>323</v>
       </c>
       <c r="G9" s="6">
         <v>23</v>
@@ -1022,7 +1061,55 @@
         <v>16</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>6</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="D10" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" s="6">
+        <v>34</v>
+      </c>
+      <c r="F10" s="6">
+        <v>33</v>
+      </c>
+      <c r="G10" s="6">
+        <v>1</v>
+      </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6">
+        <v>873</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="4">
+        <v>7</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="E11" s="6">
+        <v>10</v>
+      </c>
+      <c r="F11" s="6">
+        <v>8</v>
+      </c>
+      <c r="G11" s="6">
+        <v>2</v>
+      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6" t="s">
+        <v>38</v>
       </c>
     </row>
     <row r="17" spans="4:9" x14ac:dyDescent="0.25">
@@ -1034,7 +1121,7 @@
     </row>
     <row r="18" spans="4:9" x14ac:dyDescent="0.25">
       <c r="D18" s="5"/>
-      <c r="E18" s="16"/>
+      <c r="E18" s="15"/>
       <c r="F18" s="5"/>
       <c r="G18" s="5"/>
       <c r="H18" s="5"/>
@@ -1050,87 +1137,83 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C9452DE-FCA6-49B9-BF37-5D4D325D9379}">
-  <dimension ref="C4:J7"/>
+  <dimension ref="C4:I7"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="E6" sqref="E6:E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="15.42578125" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" customWidth="1"/>
-    <col min="10" max="10" width="22.140625" customWidth="1"/>
+    <col min="4" max="4" width="15.42578125" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:10" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="F4" s="27" t="s">
+    <row r="4" spans="3:9" ht="23.25" x14ac:dyDescent="0.35">
+      <c r="E4" s="27" t="s">
         <v>22</v>
       </c>
+      <c r="F4" s="27"/>
       <c r="G4" s="27"/>
-      <c r="H4" s="27"/>
-    </row>
-    <row r="5" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="3:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D5" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="19" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="E5" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="F5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="G5" s="17" t="s">
         <v>10</v>
       </c>
+      <c r="H5" s="17" t="s">
+        <v>11</v>
+      </c>
       <c r="I5" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="J5" s="19" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C6">
         <v>1</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="16" t="s">
-        <v>30</v>
+      <c r="D6" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="5">
+        <v>81</v>
       </c>
       <c r="F6" s="5">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="G6" s="5">
-        <v>77</v>
-      </c>
-      <c r="H6" s="5">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C7">
         <v>2</v>
       </c>
-      <c r="E7" s="22" t="s">
-        <v>29</v>
+      <c r="D7" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="E7" s="5">
+        <v>5</v>
       </c>
       <c r="F7" s="5">
         <v>5</v>
       </c>
-      <c r="G7" s="5">
-        <v>5</v>
-      </c>
-      <c r="I7" t="s">
-        <v>33</v>
+      <c r="I7" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F4:H4"/>
+    <mergeCell ref="E4:G4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1180,7 +1263,7 @@
         <v>1</v>
       </c>
       <c r="B4" s="5"/>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="13" t="s">
         <v>18</v>
       </c>
       <c r="D4" s="5">
@@ -1194,8 +1277,8 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="22" t="s">
-        <v>29</v>
+      <c r="C5" s="21" t="s">
+        <v>28</v>
       </c>
       <c r="D5" s="5">
         <v>5</v>

</xml_diff>